<commit_message>
Updating results with correct MI SEs
</commit_message>
<xml_diff>
--- a/replication/results/table5_panel1.xlsx
+++ b/replication/results/table5_panel1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>drink_def</t>
   </si>
@@ -37,25 +37,28 @@
     <t>police_report_only</t>
   </si>
   <si>
-    <t>(0.49)</t>
+    <t>(0.47)</t>
+  </si>
+  <si>
+    <t>(0.34)</t>
+  </si>
+  <si>
+    <t>any_evidence</t>
+  </si>
+  <si>
+    <t>(0.21)</t>
+  </si>
+  <si>
+    <t>(0.14)</t>
+  </si>
+  <si>
+    <t>police_report_primary</t>
   </si>
   <si>
     <t>(0.35)</t>
   </si>
   <si>
-    <t>any_evidence</t>
-  </si>
-  <si>
-    <t>(0.21)</t>
-  </si>
-  <si>
-    <t>(0.14)</t>
-  </si>
-  <si>
-    <t>police_report_primary</t>
-  </si>
-  <si>
-    <t>(0.23)</t>
+    <t>(0.27)</t>
   </si>
   <si>
     <t>bac_test_primary</t>
@@ -64,16 +67,16 @@
     <t>(0.46)</t>
   </si>
   <si>
-    <t>(0.31)</t>
+    <t>(0.28)</t>
   </si>
   <si>
     <t>multiple_imputation</t>
   </si>
   <si>
-    <t>(0.06)</t>
-  </si>
-  <si>
-    <t>(0.03)</t>
+    <t>(0.24)</t>
+  </si>
+  <si>
+    <t>(0.16)</t>
   </si>
 </sst>
 </file>
@@ -468,10 +471,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -505,13 +508,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -545,13 +548,13 @@
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>